<commit_message>
update README with notes on combinatorics and CP, update docs
also rename *.stats files to *.eval
</commit_message>
<xml_diff>
--- a/brackets/cp-sat_stats.xlsx
+++ b/brackets/cp-sat_stats.xlsx
@@ -40,7 +40,7 @@
     <t xml:space="preserve">CPU Secs</t>
   </si>
   <si>
-    <t xml:space="preserve">CPU Time</t>
+    <t xml:space="preserve">CPU (secs)</t>
   </si>
   <si>
     <t xml:space="preserve">Branch/Conflict</t>
@@ -100,6 +100,7 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -258,7 +259,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>CPU Time</c:v>
+                  <c:v>CPU (secs)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -267,7 +268,7 @@
             <a:solidFill>
               <a:srgbClr val="004586"/>
             </a:solidFill>
-            <a:ln w="28800">
+            <a:ln w="18360">
               <a:solidFill>
                 <a:srgbClr val="004586"/>
               </a:solidFill>
@@ -284,11 +285,16 @@
               <a:p>
                 <a:pPr>
                   <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
                     <a:latin typeface="Arial"/>
+                    <a:ea typeface="DejaVu Sans"/>
                   </a:defRPr>
                 </a:pPr>
               </a:p>
             </c:txPr>
+            <c:dLblPos val="r"/>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
@@ -443,17 +449,17 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="6847827"/>
-        <c:axId val="13609817"/>
+        <c:axId val="31111328"/>
+        <c:axId val="66066773"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="6847827"/>
+        <c:axId val="31111328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -470,12 +476,16 @@
           <a:p>
             <a:pPr>
               <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
                 <a:latin typeface="Arial"/>
+                <a:ea typeface="DejaVu Sans"/>
               </a:defRPr>
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="13609817"/>
+        <c:crossAx val="66066773"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -483,9 +493,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="13609817"/>
+        <c:axId val="66066773"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="7000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -498,7 +509,7 @@
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -515,13 +526,17 @@
           <a:p>
             <a:pPr>
               <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
                 <a:latin typeface="Arial"/>
+                <a:ea typeface="DejaVu Sans"/>
               </a:defRPr>
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="6847827"/>
-        <c:crosses val="autoZero"/>
+        <c:crossAx val="31111328"/>
+        <c:crossesAt val="0"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
@@ -548,7 +563,11 @@
         <a:p>
           <a:pPr>
             <a:defRPr b="0" sz="1000" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
               <a:latin typeface="Arial"/>
+              <a:ea typeface="DejaVu Sans"/>
             </a:defRPr>
           </a:pPr>
         </a:p>
@@ -573,15 +592,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>527400</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>23040</xdr:rowOff>
+      <xdr:colOff>380160</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>40320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>236520</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>11520</xdr:rowOff>
+      <xdr:colOff>503640</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>37800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -589,8 +608,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="6609960" y="1161000"/>
-        <a:ext cx="5759640" cy="3239640"/>
+        <a:off x="6462720" y="2153520"/>
+        <a:ext cx="6174000" cy="2761200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -717,7 +736,7 @@
   <dimension ref="A1:M20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H23" activeCellId="0" sqref="H23"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>